<commit_message>
IndexMapper für speicherung von Index, PatientenAttribut, OverwriteInDatenbank
</commit_message>
<xml_diff>
--- a/src/test/testDaten/test.xlsx
+++ b/src/test/testDaten/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>test 1</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>PLZ</t>
+  </si>
+  <si>
+    <t>Klaus</t>
+  </si>
+  <si>
+    <t>TEST FAILED</t>
+  </si>
+  <si>
+    <t>Kleber</t>
   </si>
 </sst>
 </file>
@@ -409,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,6 +515,23 @@
       </c>
       <c r="F5">
         <v>85841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42932</v>
+      </c>
+      <c r="F6">
+        <v>99999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Patient and Fall from Excel to DB
</commit_message>
<xml_diff>
--- a/src/test/testDaten/test.xlsx
+++ b/src/test/testDaten/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Stephan</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Geburtsdatum</t>
   </si>
   <si>
-    <t>Adresse</t>
-  </si>
-  <si>
     <t>Alternativer Name</t>
   </si>
   <si>
@@ -106,6 +103,36 @@
   </si>
   <si>
     <t>rhq qe4rz rth rwthwrtzh rtz he</t>
+  </si>
+  <si>
+    <t>Straße</t>
+  </si>
+  <si>
+    <t>E-Nummer</t>
+  </si>
+  <si>
+    <t>Befundtyp</t>
+  </si>
+  <si>
+    <t>A/1996/200591</t>
+  </si>
+  <si>
+    <t>001/00146</t>
+  </si>
+  <si>
+    <t>A/1996/200592</t>
+  </si>
+  <si>
+    <t>A/1996/200391</t>
+  </si>
+  <si>
+    <t>A/1998/200591</t>
+  </si>
+  <si>
+    <t>Hauptbefund</t>
+  </si>
+  <si>
+    <t>Nebenbefund</t>
   </si>
 </sst>
 </file>
@@ -445,26 +472,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -473,10 +500,16 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -496,10 +529,16 @@
         <v>12567</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -519,10 +558,16 @@
         <v>26451</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -539,10 +584,16 @@
         <v>34516</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -562,10 +613,16 @@
         <v>85841</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -585,11 +642,21 @@
         <v>99999</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
full DB of whole Patient, including falls
</commit_message>
<xml_diff>
--- a/src/test/testDaten/test.xlsx
+++ b/src/test/testDaten/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Stephan</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Klaus</t>
   </si>
   <si>
-    <t>TEST FAILED</t>
-  </si>
-  <si>
     <t>Kleber</t>
   </si>
   <si>
@@ -90,21 +87,6 @@
     <t>Befundtext</t>
   </si>
   <si>
-    <t>fhfdjrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdhfstjts rer zerzh  trhe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">re tgre hrth trh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rghwtreh wtrzjtrwh re rtw rwzj wrth th </t>
-  </si>
-  <si>
-    <t>rhq qe4rz rth rwthwrtzh rtz he</t>
-  </si>
-  <si>
     <t>Straße</t>
   </si>
   <si>
@@ -114,25 +96,52 @@
     <t>Befundtyp</t>
   </si>
   <si>
-    <t>A/1996/200591</t>
-  </si>
-  <si>
     <t>001/00146</t>
   </si>
   <si>
-    <t>A/1996/200592</t>
-  </si>
-  <si>
-    <t>A/1996/200391</t>
-  </si>
-  <si>
-    <t>A/1998/200591</t>
-  </si>
-  <si>
     <t>Hauptbefund</t>
   </si>
   <si>
     <t>Nebenbefund</t>
+  </si>
+  <si>
+    <t>A/2001/200592</t>
+  </si>
+  <si>
+    <t>A/2002/200591</t>
+  </si>
+  <si>
+    <t>A/2003/200391</t>
+  </si>
+  <si>
+    <t>A/2004/200591</t>
+  </si>
+  <si>
+    <t>TEST 1 update</t>
+  </si>
+  <si>
+    <t>TEST 2 kein update</t>
+  </si>
+  <si>
+    <t>A/2000/123456</t>
+  </si>
+  <si>
+    <t>Stephan Frank</t>
+  </si>
+  <si>
+    <t>Klaudis Apfel</t>
+  </si>
+  <si>
+    <t>Erika Mustermann</t>
+  </si>
+  <si>
+    <t>Max Mustermann</t>
+  </si>
+  <si>
+    <t>Klaus Kleber Excel 1</t>
+  </si>
+  <si>
+    <t>Klaus Kleber Excel 2</t>
   </si>
 </sst>
 </file>
@@ -475,38 +484,38 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -529,13 +538,13 @@
         <v>12567</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -558,13 +567,13 @@
         <v>26451</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -584,13 +593,13 @@
         <v>34516</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -613,13 +622,13 @@
         <v>85841</v>
       </c>
       <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
         <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -627,13 +636,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="1">
         <v>42932</v>
@@ -642,17 +651,43 @@
         <v>99999</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H7" s="1"/>
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1">
+        <v>42932</v>
+      </c>
+      <c r="F7">
+        <v>99999</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>